<commit_message>
Difficult to trim, but almost there
</commit_message>
<xml_diff>
--- a/inputs/beam_properties.xlsx
+++ b/inputs/beam_properties.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="mass" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t xml:space="preserve">Mass Data (Material FoR)</t>
   </si>
@@ -41,6 +41,15 @@
     <t xml:space="preserve">izz</t>
   </si>
   <si>
+    <t xml:space="preserve">xcg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ycg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zcg</t>
+  </si>
+  <si>
     <t xml:space="preserve">[-]</t>
   </si>
   <si>
@@ -50,13 +59,25 @@
     <t xml:space="preserve">[kgm]</t>
   </si>
   <si>
-    <t xml:space="preserve">inboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">outboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dihedral</t>
+    <t xml:space="preserve">[m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loutboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ldihedral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rinboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Routboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rdihedral</t>
   </si>
   <si>
     <t xml:space="preserve">boom</t>
@@ -84,6 +105,15 @@
   </si>
   <si>
     <t xml:space="preserve">eiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k34</t>
   </si>
   <si>
     <t xml:space="preserve">[Nm2]</t>
@@ -102,6 +132,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -172,7 +203,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -265,10 +296,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -300,27 +331,45 @@
       <c r="E2" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.438</v>
@@ -334,10 +383,20 @@
       <c r="E4" s="3" t="n">
         <v>0.0207</v>
       </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">0.2*(0.435 - 0.288)</f>
+        <v>0.0294</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.361</v>
@@ -351,10 +410,20 @@
       <c r="E5" s="3" t="n">
         <v>0.0184</v>
       </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">0.2*(0.435 - 0.288)</f>
+        <v>0.0294</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.428</v>
@@ -368,39 +437,148 @@
       <c r="E6" s="3" t="n">
         <v>0.0202</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">0.2*(0.395 - 0.288)</f>
+        <v>0.0214</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.07</v>
+        <v>0.438</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>2.17E-005</v>
+        <v>0.000654</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.00179</v>
+        <v>0.0134</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.00179</v>
+        <v>0.0207</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">-0.2*(0.435 - 0.288)</f>
+        <v>-0.0294</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="n">
+        <v>0.361</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0.000581</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0.0119</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>0.0184</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">-0.2*(0.435 - 0.288)</f>
+        <v>-0.0294</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.428</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>6.4E-006</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0.0131</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0.0202</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">-0.2*(0.395 - 0.288)</f>
+        <v>-0.0214</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>2.17E-005</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>0.00179</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0.00179</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="n">
         <v>0.24</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C11" s="3" t="n">
         <v>0.000171</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D11" s="3" t="n">
         <v>0.00011</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E11" s="3" t="n">
         <v>0.00597</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -422,10 +600,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -435,7 +613,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -448,50 +626,59 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>2140000</v>
@@ -513,10 +700,19 @@
       <c r="G4" s="3" t="n">
         <v>6350</v>
       </c>
+      <c r="H4" s="3" t="n">
+        <v>1540</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>-49100</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>-46.34</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>2140000</v>
@@ -538,10 +734,19 @@
       <c r="G5" s="3" t="n">
         <v>6350</v>
       </c>
+      <c r="H5" s="3" t="n">
+        <v>1540</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>-49100</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>-46.34</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>2140000</v>
@@ -563,63 +768,199 @@
       <c r="G6" s="3" t="n">
         <v>6350</v>
       </c>
+      <c r="H6" s="3" t="n">
+        <v>1540</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>-49100</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>-46.34</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="n">
-        <f aca="false">B6</f>
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="n">
         <v>2140000</v>
       </c>
       <c r="C7" s="4" t="n">
+        <f aca="false">AVERAGE(B7,E7,F7,G7)</f>
+        <v>536628</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <f aca="false">AVERAGE(B7,E7,F7,G7)</f>
+        <v>536628</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>6350</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <f aca="false">-H4</f>
+        <v>-1540</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <f aca="false">-I4</f>
+        <v>49100</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <f aca="false">-J4</f>
+        <v>46.34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>2140000</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <f aca="false">AVERAGE(B8,E8,F8,G8)</f>
+        <v>536628</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <f aca="false">AVERAGE(B8,E8,F8,G8)</f>
+        <v>536628</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>6350</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <f aca="false">-H5</f>
+        <v>-1540</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <f aca="false">-I5</f>
+        <v>49100</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <f aca="false">-J5</f>
+        <v>46.34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>2140000</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <f aca="false">AVERAGE(B9,E9,F9,G9)</f>
+        <v>536620.75</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <f aca="false">AVERAGE(B9,E9,F9,G9)</f>
+        <v>536620.75</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>79</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>6350</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <f aca="false">-H6</f>
+        <v>-1540</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <f aca="false">-I6</f>
+        <v>49100</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <f aca="false">-J6</f>
+        <v>46.34</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>2140000</v>
+      </c>
+      <c r="C10" s="4" t="n">
         <f aca="false">C6</f>
         <v>536620.75</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D10" s="4" t="n">
         <f aca="false">D6</f>
         <v>536620.75</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E10" s="4" t="n">
+        <f aca="false">10*E6</f>
+        <v>540</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <f aca="false">10*F6</f>
+        <v>790</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <f aca="false">F10</f>
+        <v>790</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>2140000</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <f aca="false">C6</f>
+        <v>536620.75</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <f aca="false">D6</f>
+        <v>536620.75</v>
+      </c>
+      <c r="E11" s="4" t="n">
         <f aca="false">E6</f>
         <v>54</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F11" s="4" t="n">
         <f aca="false">F6</f>
         <v>79</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G11" s="4" t="n">
         <f aca="false">G6</f>
         <v>6350</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="n">
-        <f aca="false">B6</f>
-        <v>2140000</v>
-      </c>
-      <c r="C8" s="4" t="n">
-        <f aca="false">C6</f>
-        <v>536620.75</v>
-      </c>
-      <c r="D8" s="4" t="n">
-        <f aca="false">D6</f>
-        <v>536620.75</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <f aca="false">E6</f>
-        <v>54</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <f aca="false">F6</f>
-        <v>79</v>
-      </c>
-      <c r="G8" s="4" t="n">
-        <f aca="false">G6</f>
-        <v>6350</v>
+      <c r="H11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -628,7 +969,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>